<commit_message>
There is an glitch in summary pipleine so it creates an empty ppt sometimes solve that tomorrow
</commit_message>
<xml_diff>
--- a/examples/Portfolio Allocation Data.xlsx
+++ b/examples/Portfolio Allocation Data.xlsx
@@ -1,123 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\OneDrive\Desktop\Big Projects\FinDeck(Excel to PPT Project)\examples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C8710C7-6BD6-4198-ACCB-CEDECF6303B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="4410" windowWidth="28800" windowHeight="15345" xr2:uid="{B7BAEB51-8A1C-4148-9730-7A2B77473D83}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4410" yWindow="4410" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
-  <si>
-    <t>Asset</t>
-  </si>
-  <si>
-    <t>Sector</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>Tech</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>Auto</t>
-  </si>
-  <si>
-    <t>TCS.NS</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>BTC-USD</t>
-  </si>
-  <si>
-    <t>Crypto</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>ETH-USD</t>
-  </si>
-  <si>
-    <t>2. Portfolio Allocation Data</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF002060"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF002060"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -141,30 +74,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -464,105 +460,395 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333648A3-7BA6-40D0-9E17-2C043E602C8F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Auto-generated Finance Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Detected PnL Sheet</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Detected Return/Price Sheet</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>File Sheet Count</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sheets</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Sample Table Preview</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2. Portfolio Allocation Data</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Unnamed: 2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Unnamed: 3</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Unnamed: 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v/>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Asset</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sector</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v/>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v/>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Auto</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v/>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TCS.NS</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v/>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BTC-USD</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Crypto</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v/>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ETH-USD</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Crypto</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col width="2.5703125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="9.140625" customWidth="1" style="1" min="2" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3">
+    <row r="1" ht="15" customHeight="1">
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>2. Portfolio Allocation Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Asset</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Sector</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3">
+    <row r="4" ht="15" customHeight="1">
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Auto</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="n">
         <v>15000</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3">
+    <row r="5" ht="15" customHeight="1">
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>TCS.NS</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3">
+    <row r="6" ht="15" customHeight="1">
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>BTC-USD</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Crypto</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="n">
         <v>8000</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="3">
+    <row r="7" ht="15" customHeight="1">
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>ETH-USD</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Crypto</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="n">
         <v>5000</v>
       </c>
     </row>

</xml_diff>